<commit_message>
Auto-committed on 2022/02/08 週二
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L2-業務作業/FacClose.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L2-業務作業/FacClose.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L2-業務作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03E5064-12B3-4F98-85CC-2E1FC38BE410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED26713-D54E-41D8-BE64-185B08A762A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -523,9 +523,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ReceiveFg</t>
-  </si>
-  <si>
     <t>領取記號</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -569,6 +566,18 @@
 6:催收戶強制執行
 7:轉列呆帳
 8:催收部分轉呆</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReceiveFg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegisteredAddress</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>雙掛號</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1163,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1464,10 +1473,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>120</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>32</v>
@@ -1477,7 +1486,7 @@
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="194.4" x14ac:dyDescent="0.3">
@@ -1560,40 +1569,40 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>14</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="17">
-        <v>8</v>
-      </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="B22" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="19">
+        <v>200</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>15</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>78</v>
+      <c r="B23" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="E23" s="17">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -1602,14 +1611,14 @@
       <c r="A24" s="19">
         <v>16</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>61</v>
+      <c r="B24" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E24" s="17">
         <v>15</v>
@@ -1621,11 +1630,11 @@
       <c r="A25" s="19">
         <v>17</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>118</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>49</v>
@@ -1640,17 +1649,17 @@
       <c r="A26" s="19">
         <v>18</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>101</v>
+      <c r="B26" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E26" s="17">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -1660,16 +1669,16 @@
         <v>19</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E27" s="17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -1679,16 +1688,16 @@
         <v>20</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="E28" s="17">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
@@ -1698,16 +1707,16 @@
         <v>21</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="E29" s="17">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
@@ -1717,16 +1726,16 @@
         <v>22</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="17">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
@@ -1735,38 +1744,36 @@
       <c r="A31" s="19">
         <v>23</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="20">
-        <v>1</v>
-      </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20" t="s">
-        <v>94</v>
-      </c>
+      <c r="B31" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="17">
+        <v>100</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>24</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="20" t="s">
@@ -1778,73 +1785,76 @@
         <v>25</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="20">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="1:7" s="18" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="G33" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>26</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F34" s="20"/>
-      <c r="G34" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7" s="18" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>27</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
+      <c r="B35" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="20">
+        <v>1</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>28</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="17">
-        <v>6</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E36" s="17"/>
       <c r="F36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1852,15 +1862,17 @@
         <v>29</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="17"/>
+        <v>32</v>
+      </c>
+      <c r="E37" s="17">
+        <v>6</v>
+      </c>
       <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1868,30 +1880,46 @@
         <v>30</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="19">
+        <v>31</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C39" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D39" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E39" s="17">
         <v>6</v>
       </c>
-      <c r="F38" s="17"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1945,7 +1973,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1989,7 +2017,7 @@
         <v>102</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2022,7 +2050,7 @@
         <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>